<commit_message>
nouvelle question et uin nouveau them
</commit_message>
<xml_diff>
--- a/data/FAQ_EXFSRI_2024.xlsx
+++ b/data/FAQ_EXFSRI_2024.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anael.delorme\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C861A731-AF1F-4663-A757-1462BAE0B3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079B29B8-3C35-4F4D-93AE-AEA493177E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
     <sheet name="Univers" sheetId="2" r:id="rId2"/>
-    <sheet name="Codification" sheetId="3" r:id="rId3"/>
-    <sheet name="Recolte" sheetId="4" r:id="rId4"/>
-    <sheet name="Sciages_Approv" sheetId="5" r:id="rId5"/>
-    <sheet name="SriProd" sheetId="9" r:id="rId6"/>
-    <sheet name="Autres activités" sheetId="6" r:id="rId7"/>
-    <sheet name="Connexes" sheetId="7" r:id="rId8"/>
-    <sheet name="Controle" sheetId="10" r:id="rId9"/>
+    <sheet name="Nouveau truc" sheetId="11" r:id="rId3"/>
+    <sheet name="Codification" sheetId="3" r:id="rId4"/>
+    <sheet name="Recolte" sheetId="4" r:id="rId5"/>
+    <sheet name="Sciages_Approv" sheetId="5" r:id="rId6"/>
+    <sheet name="SriProd" sheetId="9" r:id="rId7"/>
+    <sheet name="Autres activités" sheetId="6" r:id="rId8"/>
+    <sheet name="Connexes" sheetId="7" r:id="rId9"/>
+    <sheet name="Controle" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="266">
   <si>
     <t>Foire aux questions</t>
   </si>
@@ -1533,6 +1534,18 @@
   </si>
   <si>
     <t>si l'entreprise les coupe elle-même alors elle doit en effet les déclarer dans plaquettes forestières code 816</t>
+  </si>
+  <si>
+    <t>Ma question</t>
+  </si>
+  <si>
+    <t>Ma réponse</t>
+  </si>
+  <si>
+    <t>Biduel</t>
+  </si>
+  <si>
+    <t>machin</t>
   </si>
 </sst>
 </file>
@@ -2302,12 +2315,123 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="146.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2325,162 +2449,170 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="73.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+    <row r="5" spans="1:2" ht="73.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B5" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B6" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+    <row r="7" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B7" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B8" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+    <row r="9" spans="1:2" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B9" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B10" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+    <row r="11" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B11" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+    <row r="12" spans="1:2" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B12" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+    <row r="13" spans="1:2" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B13" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="187.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+    <row r="14" spans="1:2" ht="187.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B14" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+    <row r="15" spans="1:2" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B15" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B16" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B17" s="5" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-    </row>
-    <row r="22" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="21" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="14"/>
+    </row>
+    <row r="23" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B23" s="15" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2490,6 +2622,37 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8092A655-54B8-470A-AFAC-A816FDD68BBB}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
@@ -2605,7 +2768,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B47"/>
   <sheetViews>
@@ -2982,7 +3145,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B54"/>
   <sheetViews>
@@ -3300,7 +3463,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B97"/>
   <sheetViews>
@@ -3791,7 +3954,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -3900,7 +4063,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -4003,115 +4166,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:B17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.140625" customWidth="1"/>
-    <col min="2" max="2" width="146.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
delete subtehme empty recolte
</commit_message>
<xml_diff>
--- a/data/FAQ_EXFSRI_2024.xlsx
+++ b/data/FAQ_EXFSRI_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anael.delorme\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE336D6-CFBE-4F5D-92A7-A9FD09D85933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837407A2-2FB0-4707-88E8-5130178AB567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="991" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
     <sheet name="CONTROLES" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'RECOLTE '!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'RECOLTE '!$A$1:$D$43</definedName>
   </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="275">
   <si>
     <t>Foire aux questions</t>
   </si>
@@ -1856,13 +1856,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>2855880</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>143280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>7818120</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>1490760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2659,10 +2659,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2980,12 +2980,21 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>244</v>
+      </c>
       <c r="B23" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C23" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>244</v>
       </c>
@@ -2993,67 +3002,64 @@
         <v>261</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>244</v>
-      </c>
-      <c r="B25" t="s">
-        <v>261</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>99</v>
-      </c>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C25" s="15"/>
       <c r="D25" s="18" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>260</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>251</v>
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="18" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="201.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>251</v>
-      </c>
-      <c r="C27" s="15"/>
+        <v>240</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>102</v>
+      </c>
       <c r="D27" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="201.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>240</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>240</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>103</v>
+      <c r="C29" s="13" t="s">
+        <v>105</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -3061,167 +3067,157 @@
         <v>240</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>240</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>240</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>240</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="285" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>240</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="285" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>240</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>240</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>240</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>240</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>240</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>240</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="240" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>240</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="240" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>240</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>240</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>240</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="D44" s="13" t="s">
         <v>258</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D43" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>